<commit_message>
finished anonymous quiz implementation
</commit_message>
<xml_diff>
--- a/upload_template.xlsx
+++ b/upload_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>Course</t>
   </si>
@@ -46,6 +46,9 @@
     <t>Image</t>
   </si>
   <si>
+    <t>Anonymous</t>
+  </si>
+  <si>
     <t>Pergunta</t>
   </si>
   <si>
@@ -67,7 +70,10 @@
     <t>B</t>
   </si>
   <si>
-    <t>no_image.png</t>
+    <t>/home/joao/Pictures/Wallpapers/Diamond-TOFIX-Vector_www.FullHDWpp.com_.jpg</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -77,10 +83,10 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +100,21 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -105,15 +126,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -135,6 +158,80 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -144,98 +241,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -262,187 +275,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,6 +549,21 @@
       <top/>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -565,6 +593,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -593,201 +645,162 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -810,6 +823,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1127,22 +1143,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="C1:L84"/>
+  <dimension ref="C1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" width="8.8" style="1"/>
-    <col min="3" max="12" width="14.7" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.8" style="1"/>
+    <col min="3" max="13" width="14.7" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.8" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="26" customHeight="1"/>
     <row r="2" ht="26" customHeight="1"/>
-    <row r="3" ht="26" customHeight="1" spans="3:12">
+    <row r="3" ht="26" customHeight="1" spans="3:13">
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1173,37 +1189,43 @@
       <c r="L3" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="M3" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" ht="26" customHeight="1" spans="3:12">
+    <row r="4" ht="26" customHeight="1" spans="3:13">
       <c r="C4" s="4">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K4" s="5">
         <v>10</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1"/>

</xml_diff>

<commit_message>
made changes to firmware for new router, added quiz title to import, added 'change password' option
</commit_message>
<xml_diff>
--- a/upload_template.xlsx
+++ b/upload_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12120"/>
+    <workbookView windowWidth="15255" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
   <si>
     <t>Course</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
     <t>Question</t>
   </si>
   <si>
@@ -47,6 +50,9 @@
   </si>
   <si>
     <t>Anonymous</t>
+  </si>
+  <si>
+    <t>Título</t>
   </si>
   <si>
     <t>Pergunta</t>
@@ -81,9 +87,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -126,22 +132,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -150,9 +140,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,27 +193,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -194,22 +201,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -219,14 +210,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,7 +231,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,19 +287,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,25 +425,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -335,127 +449,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,6 +583,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -593,6 +608,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -610,23 +640,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,150 +656,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -813,6 +819,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,9 +832,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1143,89 +1149,95 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="C1:M84"/>
+  <dimension ref="B1:M84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="8.8" style="1"/>
-    <col min="3" max="13" width="14.7" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.8" style="1"/>
+    <col min="2" max="13" width="14.7" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.8" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="26" customHeight="1"/>
     <row r="2" ht="26" customHeight="1"/>
-    <row r="3" ht="26" customHeight="1" spans="3:13">
+    <row r="3" ht="26" customHeight="1" spans="2:13">
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="26" customHeight="1" spans="2:13">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="6" t="s">
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" ht="26" customHeight="1" spans="3:13">
-      <c r="C4" s="4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="5">
-        <v>10</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>18</v>
+      <c r="L4" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" ht="26" customHeight="1"/>

</xml_diff>